<commit_message>
conectando ao contoso desktop
</commit_message>
<xml_diff>
--- a/fake_invoice_data.xlsx
+++ b/fake_invoice_data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RICKINO\temp\python\invoicingBot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E00745-0A9B-4C07-9B4C-D74D60D98DCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -544,8 +550,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,11 +614,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -654,7 +668,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,9 +700,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -720,6 +752,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -895,14 +945,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -936,7 +988,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -953,7 +1005,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -964,13 +1016,13 @@
         <v>169</v>
       </c>
       <c r="D4">
-        <v>2502.93</v>
+        <v>2502.9299999999998</v>
       </c>
       <c r="E4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -987,7 +1039,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1056,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1015,13 +1067,13 @@
         <v>170</v>
       </c>
       <c r="D7">
-        <v>579.6799999999999</v>
+        <v>579.67999999999995</v>
       </c>
       <c r="E7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1038,7 +1090,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1055,7 +1107,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1124,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1141,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1106,7 +1158,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1123,7 +1175,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1140,7 +1192,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1157,7 +1209,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1174,7 +1226,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1191,7 +1243,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1208,7 +1260,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1277,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1242,7 +1294,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1259,7 +1311,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1276,7 +1328,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1287,13 +1339,13 @@
         <v>169</v>
       </c>
       <c r="D23">
-        <v>4921.48</v>
+        <v>4921.4799999999996</v>
       </c>
       <c r="E23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1310,7 +1362,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1327,7 +1379,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1344,7 +1396,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1361,7 +1413,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1430,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1395,7 +1447,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1412,7 +1464,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1429,7 +1481,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1446,7 +1498,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1457,13 +1509,13 @@
         <v>167</v>
       </c>
       <c r="D33">
-        <v>4984.4</v>
+        <v>4984.3999999999996</v>
       </c>
       <c r="E33" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1480,7 +1532,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1497,7 +1549,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1514,7 +1566,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1531,7 +1583,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1548,7 +1600,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1565,7 +1617,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1634,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1599,7 +1651,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1616,7 +1668,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1633,7 +1685,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1650,7 +1702,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1667,7 +1719,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1684,7 +1736,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1701,7 +1753,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1718,7 +1770,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1735,7 +1787,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1746,13 +1798,13 @@
         <v>168</v>
       </c>
       <c r="D50">
-        <v>2466.32</v>
+        <v>2466.3200000000002</v>
       </c>
       <c r="E50" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1769,7 +1821,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1786,7 +1838,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1803,7 +1855,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1820,7 +1872,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1831,13 +1883,13 @@
         <v>170</v>
       </c>
       <c r="D55">
-        <v>2231.72</v>
+        <v>2231.7199999999998</v>
       </c>
       <c r="E55" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1854,7 +1906,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1871,7 +1923,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1888,7 +1940,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1905,7 +1957,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1922,7 +1974,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1939,7 +1991,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1956,7 +2008,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1967,13 +2019,13 @@
         <v>169</v>
       </c>
       <c r="D63">
-        <v>2417.82</v>
+        <v>2417.8200000000002</v>
       </c>
       <c r="E63" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1990,7 +2042,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -2007,7 +2059,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -2024,7 +2076,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -2041,7 +2093,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -2058,7 +2110,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -2075,7 +2127,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2092,7 +2144,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2109,7 +2161,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2126,7 +2178,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2143,7 +2195,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2154,13 +2206,13 @@
         <v>169</v>
       </c>
       <c r="D74">
-        <v>2393.49</v>
+        <v>2393.4899999999998</v>
       </c>
       <c r="E74" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -2177,7 +2229,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2188,13 +2240,13 @@
         <v>170</v>
       </c>
       <c r="D76">
-        <v>4149.39</v>
+        <v>4149.3900000000003</v>
       </c>
       <c r="E76" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -2211,7 +2263,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2228,7 +2280,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -2245,7 +2297,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -2262,7 +2314,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -2279,7 +2331,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -2296,7 +2348,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -2313,7 +2365,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>44</v>
       </c>
@@ -2330,7 +2382,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -2347,7 +2399,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -2364,7 +2416,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -2381,7 +2433,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>35</v>
       </c>
@@ -2398,7 +2450,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>84</v>
       </c>
@@ -2415,7 +2467,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -2432,7 +2484,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>86</v>
       </c>
@@ -2449,7 +2501,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>87</v>
       </c>
@@ -2466,7 +2518,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -2483,7 +2535,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -2500,7 +2552,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>89</v>
       </c>
@@ -2517,7 +2569,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>8</v>
       </c>
@@ -2534,7 +2586,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>90</v>
       </c>
@@ -2551,7 +2603,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>74</v>
       </c>
@@ -2568,7 +2620,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>91</v>
       </c>
@@ -2585,7 +2637,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>92</v>
       </c>
@@ -2602,7 +2654,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>93</v>
       </c>
@@ -2619,7 +2671,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>94</v>
       </c>
@@ -2630,13 +2682,13 @@
         <v>168</v>
       </c>
       <c r="D102">
-        <v>4706.31</v>
+        <v>4706.3100000000004</v>
       </c>
       <c r="E102" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -2653,7 +2705,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>95</v>
       </c>
@@ -2664,13 +2716,13 @@
         <v>171</v>
       </c>
       <c r="D104">
-        <v>4677.89</v>
+        <v>4677.8900000000003</v>
       </c>
       <c r="E104" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>96</v>
       </c>
@@ -2687,7 +2739,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
@@ -2704,7 +2756,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>98</v>
       </c>
@@ -2721,7 +2773,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -2732,13 +2784,13 @@
         <v>171</v>
       </c>
       <c r="D108">
-        <v>4304.94</v>
+        <v>4304.9399999999996</v>
       </c>
       <c r="E108" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>100</v>
       </c>
@@ -2755,7 +2807,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -2772,7 +2824,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -2789,7 +2841,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>102</v>
       </c>
@@ -2806,7 +2858,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>80</v>
       </c>
@@ -2823,7 +2875,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>59</v>
       </c>
@@ -2840,7 +2892,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>24</v>
       </c>
@@ -2857,7 +2909,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>103</v>
       </c>
@@ -2874,7 +2926,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -2891,7 +2943,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>105</v>
       </c>
@@ -2908,7 +2960,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>106</v>
       </c>
@@ -2925,7 +2977,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>21</v>
       </c>
@@ -2942,7 +2994,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>15</v>
       </c>
@@ -2959,7 +3011,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -2976,7 +3028,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>108</v>
       </c>
@@ -2987,13 +3039,13 @@
         <v>171</v>
       </c>
       <c r="D123">
-        <v>552.45</v>
+        <v>552.45000000000005</v>
       </c>
       <c r="E123" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>109</v>
       </c>
@@ -3010,7 +3062,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>110</v>
       </c>
@@ -3021,13 +3073,13 @@
         <v>171</v>
       </c>
       <c r="D125">
-        <v>4799.77</v>
+        <v>4799.7700000000004</v>
       </c>
       <c r="E125" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>111</v>
       </c>
@@ -3044,7 +3096,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>112</v>
       </c>
@@ -3061,7 +3113,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>113</v>
       </c>
@@ -3072,13 +3124,13 @@
         <v>171</v>
       </c>
       <c r="D128">
-        <v>782.5700000000001</v>
+        <v>782.57</v>
       </c>
       <c r="E128" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -3095,7 +3147,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>114</v>
       </c>
@@ -3112,7 +3164,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>115</v>
       </c>
@@ -3129,7 +3181,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>116</v>
       </c>
@@ -3146,7 +3198,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>117</v>
       </c>
@@ -3163,7 +3215,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>51</v>
       </c>
@@ -3180,7 +3232,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>118</v>
       </c>
@@ -3197,7 +3249,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>119</v>
       </c>
@@ -3214,7 +3266,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>120</v>
       </c>
@@ -3231,7 +3283,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>121</v>
       </c>
@@ -3248,7 +3300,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>122</v>
       </c>
@@ -3265,7 +3317,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>123</v>
       </c>
@@ -3282,7 +3334,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>124</v>
       </c>
@@ -3293,13 +3345,13 @@
         <v>170</v>
       </c>
       <c r="D141">
-        <v>4352.44</v>
+        <v>4352.4399999999996</v>
       </c>
       <c r="E141" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>24</v>
       </c>
@@ -3310,13 +3362,13 @@
         <v>168</v>
       </c>
       <c r="D142">
-        <v>641.05</v>
+        <v>641.04999999999995</v>
       </c>
       <c r="E142" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>115</v>
       </c>
@@ -3333,7 +3385,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>125</v>
       </c>
@@ -3350,7 +3402,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>126</v>
       </c>
@@ -3367,7 +3419,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>127</v>
       </c>
@@ -3384,7 +3436,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>128</v>
       </c>
@@ -3401,7 +3453,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>129</v>
       </c>
@@ -3418,7 +3470,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>130</v>
       </c>
@@ -3435,7 +3487,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>131</v>
       </c>
@@ -3452,7 +3504,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>132</v>
       </c>
@@ -3469,7 +3521,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>123</v>
       </c>
@@ -3486,7 +3538,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>133</v>
       </c>
@@ -3503,7 +3555,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>51</v>
       </c>
@@ -3514,13 +3566,13 @@
         <v>169</v>
       </c>
       <c r="D154">
-        <v>589.5700000000001</v>
+        <v>589.57000000000005</v>
       </c>
       <c r="E154" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>84</v>
       </c>
@@ -3537,7 +3589,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>134</v>
       </c>
@@ -3554,7 +3606,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>87</v>
       </c>
@@ -3565,13 +3617,13 @@
         <v>171</v>
       </c>
       <c r="D157">
-        <v>1104.65</v>
+        <v>1104.6500000000001</v>
       </c>
       <c r="E157" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>135</v>
       </c>
@@ -3588,7 +3640,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>82</v>
       </c>
@@ -3605,7 +3657,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>136</v>
       </c>
@@ -3622,7 +3674,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>137</v>
       </c>
@@ -3639,7 +3691,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>138</v>
       </c>
@@ -3656,7 +3708,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>85</v>
       </c>
@@ -3673,7 +3725,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>139</v>
       </c>
@@ -3690,7 +3742,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>140</v>
       </c>
@@ -3707,7 +3759,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>100</v>
       </c>
@@ -3724,7 +3776,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>117</v>
       </c>
@@ -3741,7 +3793,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>141</v>
       </c>
@@ -3758,7 +3810,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>142</v>
       </c>
@@ -3775,7 +3827,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>143</v>
       </c>
@@ -3792,7 +3844,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>144</v>
       </c>
@@ -3809,7 +3861,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>145</v>
       </c>
@@ -3820,13 +3872,13 @@
         <v>171</v>
       </c>
       <c r="D172">
-        <v>1182.39</v>
+        <v>1182.3900000000001</v>
       </c>
       <c r="E172" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>43</v>
       </c>
@@ -3843,7 +3895,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>132</v>
       </c>
@@ -3860,7 +3912,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>146</v>
       </c>
@@ -3871,13 +3923,13 @@
         <v>168</v>
       </c>
       <c r="D175">
-        <v>4174.85</v>
+        <v>4174.8500000000004</v>
       </c>
       <c r="E175" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>95</v>
       </c>
@@ -3888,13 +3940,13 @@
         <v>167</v>
       </c>
       <c r="D176">
-        <v>2080.7</v>
+        <v>2080.6999999999998</v>
       </c>
       <c r="E176" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>147</v>
       </c>
@@ -3911,7 +3963,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>148</v>
       </c>
@@ -3928,7 +3980,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>103</v>
       </c>
@@ -3945,7 +3997,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>149</v>
       </c>
@@ -3962,7 +4014,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>120</v>
       </c>
@@ -3979,7 +4031,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>150</v>
       </c>
@@ -3996,7 +4048,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>151</v>
       </c>
@@ -4013,7 +4065,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>152</v>
       </c>
@@ -4030,7 +4082,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>153</v>
       </c>
@@ -4047,7 +4099,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>154</v>
       </c>
@@ -4064,7 +4116,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>122</v>
       </c>
@@ -4081,7 +4133,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>42</v>
       </c>
@@ -4098,7 +4150,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>94</v>
       </c>
@@ -4109,13 +4161,13 @@
         <v>170</v>
       </c>
       <c r="D189">
-        <v>4783.65</v>
+        <v>4783.6499999999996</v>
       </c>
       <c r="E189" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>152</v>
       </c>
@@ -4132,7 +4184,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>155</v>
       </c>
@@ -4149,7 +4201,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>156</v>
       </c>
@@ -4166,7 +4218,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>157</v>
       </c>
@@ -4183,7 +4235,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>75</v>
       </c>
@@ -4194,13 +4246,13 @@
         <v>171</v>
       </c>
       <c r="D194">
-        <v>4682.1</v>
+        <v>4682.1000000000004</v>
       </c>
       <c r="E194" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>158</v>
       </c>
@@ -4217,7 +4269,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>151</v>
       </c>
@@ -4234,7 +4286,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>144</v>
       </c>
@@ -4251,7 +4303,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>159</v>
       </c>
@@ -4268,7 +4320,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>160</v>
       </c>
@@ -4285,7 +4337,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>161</v>
       </c>
@@ -4302,7 +4354,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>34</v>
       </c>
@@ -4313,7 +4365,7 @@
         <v>171</v>
       </c>
       <c r="D201">
-        <v>2383.45</v>
+        <v>2383.4499999999998</v>
       </c>
       <c r="E201" t="s">
         <v>174</v>

</xml_diff>